<commit_message>
xmlwriter: fix _xHHHH_ escapes greater than _x00FF_
</commit_message>
<xml_diff>
--- a/tests/input/shared_strings02.xlsx
+++ b/tests/input/shared_strings02.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>_</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>__x005F_x0000__</t>
+  </si>
+  <si>
+    <t>_x005F_x597D_</t>
+  </si>
+  <si>
+    <t>_x005F_x597d_</t>
+  </si>
+  <si>
+    <t>_x597G_</t>
+  </si>
+  <si>
+    <t>_x_x_x</t>
   </si>
 </sst>
 </file>
@@ -387,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -463,6 +475,26 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>